<commit_message>
feat: update enrollment form
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/no_contact.xlsx
+++ b/config/itech-aurum/forms/app/no_contact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DA64A0-17FD-A743-B367-1D0ADF188872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1CD367-AD18-F248-A883-1E8EF563C7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,101 +170,101 @@
     <t>n_header</t>
   </si>
   <si>
+    <t>select_one yes_no_unknown</t>
+  </si>
+  <si>
+    <t>client_ok</t>
+  </si>
+  <si>
+    <t>Is VMMC Client okay?</t>
+  </si>
+  <si>
+    <t>additional_notes_text</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>if(${client_ok}="unknown", "Trace client and add additional notes ", if(${client_ok}="no","Review Client and add additional notes", "Please add additional notes"))</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>additional_notes</t>
+  </si>
+  <si>
+    <t>${additional_notes_text}</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yes_no_unknown</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>formId</t>
+  </si>
+  <si>
+    <t>default_language</t>
+  </si>
+  <si>
+    <t>No Contact</t>
+  </si>
+  <si>
+    <t>no_contact</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>instance::tag</t>
+  </si>
+  <si>
+    <t>Client reached and reports no concerns (no follow-up needed)</t>
+  </si>
+  <si>
+    <t>Client reached and needs in-person review (generate the Task for site-based in-person review)</t>
+  </si>
+  <si>
+    <t>Client not reached (generates Task for site tracing)</t>
+  </si>
+  <si>
     <t>&lt;h4 style="color: #337ab7;"&gt;If there is no sms text response from the client on day 8, nurse makes contact via phone to the client and/or the next kin to find out if they are okay, this form reports on the outcomes of the actions of the nurse and can lead to either&lt;br/&gt;
-1) a client has been reached and is ok
-2) a client is has been reached and needs review
-3) client has not been reached
+1) a client reached and is ok
+2) a client reached and NEEDS in-person  review
+3) client not reached, needs tracing
 &lt;/h4&gt;</t>
-  </si>
-  <si>
-    <t>select_one yes_no_unknown</t>
-  </si>
-  <si>
-    <t>client_ok</t>
-  </si>
-  <si>
-    <t>Is VMMC Client okay?</t>
-  </si>
-  <si>
-    <t>additional_notes_text</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>if(${client_ok}="unknown", "Trace client and add additional notes ", if(${client_ok}="no","Review Client and add additional notes", "Please add additional notes"))</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>additional_notes</t>
-  </si>
-  <si>
-    <t>${additional_notes_text}</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>yes_no_unknown</t>
-  </si>
-  <si>
-    <t>Yes, no follow-up needed</t>
-  </si>
-  <si>
-    <t>No, client needs care</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>Unknown, client not reached</t>
-  </si>
-  <si>
-    <t>form_title</t>
-  </si>
-  <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>style</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>instance_name</t>
-  </si>
-  <si>
-    <t>formId</t>
-  </si>
-  <si>
-    <t>default_language</t>
-  </si>
-  <si>
-    <t>No Contact</t>
-  </si>
-  <si>
-    <t>no_contact</t>
-  </si>
-  <si>
-    <t>pages</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>instance::tag</t>
   </si>
 </sst>
 </file>
@@ -687,9 +687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -740,7 +740,7 @@
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1031,7 +1031,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="16" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>50</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1098,7 +1098,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>44</v>
@@ -1106,14 +1106,14 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -1133,18 +1133,18 @@
     </row>
     <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -2185,7 +2185,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2199,7 +2199,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -2215,35 +2215,35 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>61</v>
-      </c>
       <c r="C5" s="18" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3257,31 +3257,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>68</v>
       </c>
       <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
@@ -3303,29 +3303,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C2" s="26">
         <v>43896</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>

</xml_diff>

<commit_message>
feat: add descriptions to no contact options
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/no_contact.xlsx
+++ b/config/itech-aurum/forms/app/no_contact.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221BD50B-FC71-2E48-B923-A47619076A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC2A9A9-81FB-3444-AA11-A275A8E7F70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-2900" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-2900" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -245,19 +245,10 @@
     <t>Client reached by phone or SMS and reports no concerns (no follow-up needed)</t>
   </si>
   <si>
-    <t>Client reached by phone or SMS and needs in-person review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client traced by SMS or phone but not found </t>
-  </si>
-  <si>
     <t>yes_ok</t>
   </si>
   <si>
     <t>yes_not_ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client has already been seen at the clinic </t>
   </si>
   <si>
     <t>yes_visited</t>
@@ -268,6 +259,15 @@
   <si>
     <t>&lt;h4 style="color: #337ab7;"&gt;Hub Nurse Completes this task form for minors and adults who appear to have no interaction via SMS with the team post MC on day 3 (minors) and day 8 (adults) respectively.
 &lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t>Client reached by phone or SMS and needs in-person review (refer for care)</t>
+  </si>
+  <si>
+    <t>Client traced by SMS or phone but not found (generate tracing task)</t>
+  </si>
+  <si>
+    <t>Client has already been seen at the clinic (no follow-up needed)</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D20" sqref="D20:D25"/>
     </sheetView>
@@ -1044,7 +1044,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1114,7 +1114,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="5"/>
@@ -2156,9 +2156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C972"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2191,7 +2191,7 @@
         <v>54</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>71</v>
@@ -2202,10 +2202,10 @@
         <v>54</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2216,7 +2216,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2224,10 +2224,10 @@
         <v>54</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>